<commit_message>
added units column to variable descriptions
</commit_message>
<xml_diff>
--- a/nessusOut2_VariableDescription.xlsx
+++ b/nessusOut2_VariableDescription.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EACE-Precision-1\Google Drive\WORK\PROJECTS\AnkleSprains\code\git\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EACE-Precision-1\Google Drive\WORK\PROJECTS\AnkleSprains\code\git\anklesprain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E1C5EE6-AF28-4A5D-9F0A-21C59D3A0D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8DBE428-A817-448A-8E6A-0B4E88961731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29430" yWindow="2040" windowWidth="23235" windowHeight="11505" xr2:uid="{E5FC99BB-6E4D-401C-942D-FDD5CEC1AC25}"/>
+    <workbookView xWindow="3390" yWindow="2265" windowWidth="22830" windowHeight="12345" xr2:uid="{E5FC99BB-6E4D-401C-942D-FDD5CEC1AC25}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="61">
   <si>
     <t>time</t>
   </si>
@@ -132,9 +132,6 @@
     <t>talus_r_Oz</t>
   </si>
   <si>
-    <t>Anterior +X. Predicted foot-platform contact force, applied to COM of calcn_r, In ground reference frame</t>
-  </si>
-  <si>
     <t>Predicted moment due to foot-floor contact, applied to COM of calcn_r. In ground reference frame. Orignally from ForceReporter_forces.sto, foot_floor_r_calcn_r_torque_X</t>
   </si>
   <si>
@@ -171,7 +168,46 @@
     <t>joint angular velocity about subtalar helical axis</t>
   </si>
   <si>
-    <t>Each of the below are x3 translations, x3 rotations (XYZ body-fixed Euler angles) for the named segment with respect to ground. Originally from BodyKinematics_pos_global.sto</t>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Degrees</t>
+  </si>
+  <si>
+    <t>Degrees / second</t>
+  </si>
+  <si>
+    <t>meters</t>
+  </si>
+  <si>
+    <t>X translation between global origin and body COM. Originally from BodyKinematics_pos_global.sto</t>
+  </si>
+  <si>
+    <t>Y translation between global origin and body COM. Originally from BodyKinematics_pos_global.sto</t>
+  </si>
+  <si>
+    <t>Z translation between global origin and body COM. Originally from BodyKinematics_pos_global.sto</t>
+  </si>
+  <si>
+    <t>Euler body-fixed rotation (XYZ sequence) between global frame, and body frame. Originally from BodyKinematics_pos_global.sto</t>
+  </si>
+  <si>
+    <t>" same as for tibia</t>
+  </si>
+  <si>
+    <t>seconds</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>N-m</t>
   </si>
 </sst>
 </file>
@@ -495,7 +531,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -610,6 +646,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -655,10 +700,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1014,246 +1060,385 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5F9FF05-2DA7-4523-9781-F9CB2DF3133C}">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.28515625" customWidth="1"/>
-    <col min="2" max="2" width="46.5703125" customWidth="1"/>
-    <col min="3" max="5" width="9" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="46.5703125" customWidth="1"/>
+    <col min="4" max="6" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="2" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="2" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="B19" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="B20" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="B21" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="B22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="B23" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="B24" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="B25" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="B26" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="B27" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="B28" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="B29" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="B30" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="B31" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="B32" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="B33" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="B34" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="B35" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>34</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>